<commit_message>
Added Grid and docker support
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SeleniumTestAutomationFramework\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{569AD40A-9683-4C30-AED1-B79BE2BEECD6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E361E0-E15C-4114-9002-7F95CE7D7EA1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{68AB1946-3CB0-46DB-8201-2DC0F001D980}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
   <si>
     <t>TestName</t>
   </si>
@@ -37,12 +37,6 @@
     <t>RunFlag</t>
   </si>
   <si>
-    <t>test the login functionality</t>
-  </si>
-  <si>
-    <t>test homepage</t>
-  </si>
-  <si>
     <t>priority</t>
   </si>
   <si>
@@ -55,31 +49,28 @@
     <t>yes</t>
   </si>
   <si>
-    <t>loginTest</t>
-  </si>
-  <si>
-    <t>applyLeave</t>
-  </si>
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>admin123</t>
-  </si>
-  <si>
     <t>browser</t>
   </si>
   <si>
     <t>chrome</t>
   </si>
   <si>
-    <t>firefox</t>
+    <t>productName</t>
+  </si>
+  <si>
+    <t>iphone SE</t>
+  </si>
+  <si>
+    <t>searchProductTest1</t>
+  </si>
+  <si>
+    <t>searchProductTest2</t>
+  </si>
+  <si>
+    <t>Search Functionality</t>
+  </si>
+  <si>
+    <t>Oneplus 9R</t>
   </si>
 </sst>
 </file>
@@ -123,12 +114,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,7 +438,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -466,44 +458,44 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -514,22 +506,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6C74BD3-82AF-4315-94B7-6DEB581E2FB2}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.6640625" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -537,50 +528,42 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="D3" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added ELK support and Docker Compose
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SeleniumTestAutomationFramework\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E361E0-E15C-4114-9002-7F95CE7D7EA1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510DC6BC-3171-48AF-A6C0-D24994BF99F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{68AB1946-3CB0-46DB-8201-2DC0F001D980}"/>
   </bookViews>
@@ -52,25 +52,25 @@
     <t>browser</t>
   </si>
   <si>
+    <t>productName</t>
+  </si>
+  <si>
+    <t>iphone SE</t>
+  </si>
+  <si>
+    <t>searchProductTest1</t>
+  </si>
+  <si>
+    <t>searchProductTest2</t>
+  </si>
+  <si>
+    <t>Search Functionality</t>
+  </si>
+  <si>
+    <t>Oneplus 9R</t>
+  </si>
+  <si>
     <t>chrome</t>
-  </si>
-  <si>
-    <t>productName</t>
-  </si>
-  <si>
-    <t>iphone SE</t>
-  </si>
-  <si>
-    <t>searchProductTest1</t>
-  </si>
-  <si>
-    <t>searchProductTest2</t>
-  </si>
-  <si>
-    <t>Search Functionality</t>
-  </si>
-  <si>
-    <t>Oneplus 9R</t>
   </si>
 </sst>
 </file>
@@ -466,10 +466,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -483,10 +483,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -509,7 +509,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -531,35 +531,35 @@
         <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>